<commit_message>
Gene Banks Exapnded 업데이트
</commit_message>
<xml_diff>
--- a/Data/Gene Banks Exapnded - 3138968978/3138968978.xlsx
+++ b/Data/Gene Banks Exapnded - 3138968978/3138968978.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Gene Banks Exapnded - 3138968978\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A472650-A977-46AC-8C8C-48D7CE5CE5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C22F1C0-4087-44C0-A89B-7AB8A4C00E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240128" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240210" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +32,180 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>강석진</author>
+  </authors>
+  <commentList>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{4E80D0D2-A5F6-41C4-95E2-CF9CA9273C9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>모드로</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>유전자팩</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>보관</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>한도가</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 4</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>→</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>8</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>로</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>바뀜</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -100,15 +272,31 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>바닐라 번역 차용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>이 건물은 유전자 조합기 근처에 배치되었을 시, 변형이식체를 만드는데 필요한 유전자묶음을 저장하고 제공합니다. 유전자 저장고가 더 많이 지어질 수록 더 많은 양의 유전자묶음을 저장 할 수 있습니다.\n\n전력이 공급된동안 유전자 저장고는 유전자묶음의 부패를 방지하고 피해를 천천히 복구합니다.\n\n20개의 유전자묶음 슬롯을 가지고 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>이 건물은 유전자 조합기 근처에 배치되었을 시, 변형이식체를 만드는데 필요한 유전자묶음을 저장하고 제공합니다. 유전자 저장고가 더 많이 지어질 수록 더 많은 양의 유전자묶음을 저장 할 수 있습니다.\n\n전력이 공급된동안 유전자 저장고는 유전자묶음의 부패를 방지하고 피해를 천천히 복구합니다.\n\n48개의 유전자묶음 슬롯을 가지고 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+GeneBank.description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>This building can store genepacks and make them usable to create new xenogerms, when placed near a gene assembler. Large gene libraries require many gene banks.\n\nWhen powered, gene banks prevent genepacks from deteriorating and will slowly repair deterioration.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 건물은 유전자 조합기 근처에 배치되었을 시, 변형이식체를 만드는데 필요한 유전자묶음을 저장하고 제공합니다. 유전자 저장고가 더 많이 지어질 수록 더 많은 양의 유전자묶음을 저장 할 수 있습니다.\n\n전력이 공급된동안 유전자 저장고는 유전자묶음의 부패를 방지하고 피해를 천천히 복구합니다.\n\n8개의 유전자묶음 슬롯을 가지고 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닐라 유전자 저장고</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GeneBank.description</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -116,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,6 +328,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -492,11 +695,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -507,7 +710,7 @@
     <col min="4" max="4" width="29.26953125" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="40.1796875" style="1" customWidth="1"/>
     <col min="6" max="6" width="98.08984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -530,9 +733,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -565,7 +766,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -600,11 +801,32 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>